<commit_message>
RA html changes| added sample query
</commit_message>
<xml_diff>
--- a/server/files/Testing.xlsx
+++ b/server/files/Testing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sadafnajam/Desktop/KnowledgeBase/server/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sekho\KnowledgeBase\server\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CABE7C6-A89B-1848-BE06-8F92AB5ED966}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4127839F-BA42-42C3-AB11-5CE09C0E9F88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15340" xr2:uid="{6011F1DF-94F9-E246-B49A-717FD9EB4B7F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{6011F1DF-94F9-E246-B49A-717FD9EB4B7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -139,12 +137,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -557,274 +555,274 @@
   <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="125" style="1" customWidth="1"/>
     <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A5" s="3"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A7" s="3"/>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A8" s="3"/>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A9" s="3"/>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A10" s="3"/>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A11" s="3"/>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A12" s="3"/>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A13" s="3"/>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A14" s="3"/>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A15" s="3"/>
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="C20" s="4"/>
-    </row>
-    <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="C21" s="4"/>
-    </row>
-    <row r="22" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="C22" s="4"/>
-    </row>
-    <row r="23" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="C23" s="4"/>
-    </row>
-    <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="C24" s="4"/>
-    </row>
-    <row r="25" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="C25" s="4"/>
-    </row>
-    <row r="26" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="C26" s="4"/>
-    </row>
-    <row r="27" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="C27" s="4"/>
-    </row>
-    <row r="28" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="C28" s="4"/>
-    </row>
-    <row r="29" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="C29" s="4"/>
-    </row>
-    <row r="30" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="C30" s="4"/>
-    </row>
-    <row r="31" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="C31" s="4"/>
-    </row>
-    <row r="32" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="C32" s="4"/>
-    </row>
-    <row r="33" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="C33" s="4"/>
-    </row>
-    <row r="34" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A17" s="3"/>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A18" s="3"/>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A19" s="3"/>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A20" s="3"/>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A21" s="3"/>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A22" s="4"/>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A23" s="4"/>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A24" s="4"/>
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A25" s="4"/>
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A26" s="4"/>
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A27" s="4"/>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A28" s="4"/>
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A29" s="4"/>
+      <c r="C29" s="3"/>
+    </row>
+    <row r="30" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A30" s="4"/>
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A31" s="4"/>
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A32" s="4"/>
+      <c r="C32" s="3"/>
+    </row>
+    <row r="33" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A33" s="4"/>
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A34" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="4" t="s">
+      <c r="B34" s="5"/>
+      <c r="C34" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="C35" s="4"/>
-    </row>
-    <row r="36" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="C36" s="4"/>
-    </row>
-    <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="C37" s="4"/>
-    </row>
-    <row r="38" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="C38" s="4"/>
-    </row>
-    <row r="39" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="C39" s="4"/>
-    </row>
-    <row r="40" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="C40" s="4"/>
-    </row>
-    <row r="41" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="C41" s="4"/>
-    </row>
-    <row r="42" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="C42" s="4"/>
-    </row>
-    <row r="43" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="C43" s="4"/>
+    <row r="35" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A35" s="4"/>
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A36" s="4"/>
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A37" s="4"/>
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A38" s="4"/>
+      <c r="C38" s="3"/>
+    </row>
+    <row r="39" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A39" s="4"/>
+      <c r="C39" s="3"/>
+    </row>
+    <row r="40" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A40" s="4"/>
+      <c r="C40" s="3"/>
+    </row>
+    <row r="41" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A41" s="4"/>
+      <c r="C41" s="3"/>
+    </row>
+    <row r="42" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A42" s="4"/>
+      <c r="C42" s="3"/>
+    </row>
+    <row r="43" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A43" s="4"/>
+      <c r="C43" s="3"/>
       <c r="E43" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="C44" s="4"/>
-    </row>
-    <row r="45" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="C45" s="4"/>
-    </row>
-    <row r="46" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="C46" s="4"/>
-    </row>
-    <row r="47" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="C47" s="4"/>
-    </row>
-    <row r="48" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="C48" s="4"/>
-    </row>
-    <row r="49" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="C49" s="4"/>
-    </row>
-    <row r="50" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
-      <c r="C50" s="4"/>
-    </row>
-    <row r="51" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
-      <c r="C51" s="4"/>
-    </row>
-    <row r="52" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A52" s="5"/>
-      <c r="C52" s="4"/>
-    </row>
-    <row r="53" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A53" s="5"/>
-      <c r="C53" s="4"/>
-    </row>
-    <row r="54" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A54" s="5"/>
-      <c r="C54" s="4"/>
-    </row>
-    <row r="55" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A55" s="5"/>
-      <c r="C55" s="4"/>
-    </row>
-    <row r="56" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A56" s="5"/>
-      <c r="C56" s="4"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="5"/>
+    <row r="44" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A44" s="4"/>
+      <c r="C44" s="3"/>
+    </row>
+    <row r="45" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A45" s="4"/>
+      <c r="C45" s="3"/>
+    </row>
+    <row r="46" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A46" s="4"/>
+      <c r="C46" s="3"/>
+    </row>
+    <row r="47" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A47" s="4"/>
+      <c r="C47" s="3"/>
+    </row>
+    <row r="48" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A48" s="4"/>
+      <c r="C48" s="3"/>
+    </row>
+    <row r="49" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A49" s="4"/>
+      <c r="C49" s="3"/>
+    </row>
+    <row r="50" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A50" s="4"/>
+      <c r="C50" s="3"/>
+    </row>
+    <row r="51" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A51" s="4"/>
+      <c r="C51" s="3"/>
+    </row>
+    <row r="52" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A52" s="4"/>
+      <c r="C52" s="3"/>
+    </row>
+    <row r="53" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A53" s="4"/>
+      <c r="C53" s="3"/>
+    </row>
+    <row r="54" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A54" s="4"/>
+      <c r="C54" s="3"/>
+    </row>
+    <row r="55" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A55" s="4"/>
+      <c r="C55" s="3"/>
+    </row>
+    <row r="56" spans="1:3" ht="21" x14ac:dyDescent="0.5">
+      <c r="A56" s="4"/>
+      <c r="C56" s="3"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>